<commit_message>
respiration updated 4 12 2023
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Physiology/Respiration/Resp_counts.xlsx
+++ b/RAnalysis/Data/Physiology/Respiration/Resp_counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Airradians_parentXoffspring_OA\RAnalysis\Data\Physiology\Respiration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C7A5EE3-ECF5-4CE3-A21E-790E20F38C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B920092-C546-4F3B-A61A-ACB54D6C7811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7CFDEFA2-7D68-41F2-995D-5662DC8D953D}"/>
+    <workbookView xWindow="29370" yWindow="-16200" windowWidth="14610" windowHeight="7845" xr2:uid="{7CFDEFA2-7D68-41F2-995D-5662DC8D953D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -429,7 +429,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,7 +465,7 @@
         <v>16</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(B2:D2)</f>
+        <f t="shared" ref="E2:E19" si="0">AVERAGE(B2:D2)</f>
         <v>16</v>
       </c>
     </row>
@@ -483,7 +483,7 @@
         <v>16</v>
       </c>
       <c r="E3">
-        <f>AVERAGE(B3:D3)</f>
+        <f t="shared" si="0"/>
         <v>12.333333333333334</v>
       </c>
     </row>
@@ -501,7 +501,7 @@
         <v>15</v>
       </c>
       <c r="E4">
-        <f>AVERAGE(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>11.333333333333334</v>
       </c>
     </row>
@@ -519,7 +519,7 @@
         <v>12</v>
       </c>
       <c r="E5">
-        <f>AVERAGE(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>10.333333333333334</v>
       </c>
     </row>
@@ -537,7 +537,7 @@
         <v>15</v>
       </c>
       <c r="E6">
-        <f>AVERAGE(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
@@ -555,7 +555,7 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <f>AVERAGE(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -573,7 +573,7 @@
         <v>15</v>
       </c>
       <c r="E8">
-        <f>AVERAGE(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>17.666666666666668</v>
       </c>
     </row>
@@ -591,7 +591,7 @@
         <v>24</v>
       </c>
       <c r="E9">
-        <f>AVERAGE(B9:D9)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -609,7 +609,7 @@
         <v>13</v>
       </c>
       <c r="E10">
-        <f>AVERAGE(B10:D10)</f>
+        <f t="shared" si="0"/>
         <v>11.666666666666666</v>
       </c>
     </row>
@@ -627,7 +627,7 @@
         <v>14</v>
       </c>
       <c r="E11">
-        <f>AVERAGE(B11:D11)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
@@ -645,7 +645,7 @@
         <v>11</v>
       </c>
       <c r="E12">
-        <f>AVERAGE(B12:D12)</f>
+        <f t="shared" si="0"/>
         <v>13.666666666666666</v>
       </c>
     </row>
@@ -663,7 +663,7 @@
         <v>15</v>
       </c>
       <c r="E13">
-        <f>AVERAGE(B13:D13)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
@@ -681,7 +681,7 @@
         <v>18</v>
       </c>
       <c r="E14">
-        <f>AVERAGE(B14:D14)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -699,7 +699,7 @@
         <v>14</v>
       </c>
       <c r="E15">
-        <f>AVERAGE(B15:D15)</f>
+        <f t="shared" si="0"/>
         <v>13.666666666666666</v>
       </c>
     </row>
@@ -717,7 +717,7 @@
         <v>12</v>
       </c>
       <c r="E16">
-        <f>AVERAGE(B16:D16)</f>
+        <f t="shared" si="0"/>
         <v>12.333333333333334</v>
       </c>
     </row>
@@ -735,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="E17">
-        <f>AVERAGE(B17:D17)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -753,7 +753,7 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <f>AVERAGE(B18:D18)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -771,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="E19">
-        <f>AVERAGE(B19:D19)</f>
+        <f t="shared" si="0"/>
         <v>9.6666666666666661</v>
       </c>
     </row>

</xml_diff>